<commit_message>
combined and corrected df
</commit_message>
<xml_diff>
--- a/Iran-Mazandaran-Javaherdeh site.xlsx
+++ b/Iran-Mazandaran-Javaherdeh site.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TRU\Iran_data\CSV\Iran_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28F1E77E-AE6E-4114-9967-B62BBFEBFAA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EC4FE8-87B7-4C9B-ACC0-68946D741827}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Excolure area" sheetId="3" r:id="rId1"/>
@@ -38,12 +38,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>MRT Pack 20 DVDs</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="646">
   <si>
     <t>UPS Location (GPS coordinates)</t>
   </si>
@@ -7353,12 +7353,31 @@
       <t xml:space="preserve"> DC.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Anagallis arvensis L.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>vensis L.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7473,6 +7492,17 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -7691,7 +7721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -7890,8 +7920,11 @@
     <xf numFmtId="2" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -7900,31 +7933,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -7938,23 +7950,41 @@
     <xf numFmtId="15" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -7966,6 +7996,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8001,18 +8043,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8350,10 +8381,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="G11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
@@ -8372,312 +8403,312 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
     </row>
     <row r="2" spans="1:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
       <c r="F2" s="61"/>
       <c r="G2" s="61"/>
-      <c r="H2" s="88" t="s">
+      <c r="H2" s="82" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
-      <c r="V2" s="89"/>
-      <c r="W2" s="89"/>
-      <c r="X2" s="89"/>
-      <c r="Y2" s="89"/>
-      <c r="Z2" s="89"/>
-      <c r="AA2" s="89"/>
-      <c r="AB2" s="89"/>
-      <c r="AC2" s="89"/>
-      <c r="AD2" s="89"/>
-      <c r="AE2" s="90"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="83"/>
+      <c r="W2" s="83"/>
+      <c r="X2" s="83"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="83"/>
+      <c r="AA2" s="83"/>
+      <c r="AB2" s="83"/>
+      <c r="AC2" s="83"/>
+      <c r="AD2" s="83"/>
+      <c r="AE2" s="84"/>
     </row>
     <row r="3" spans="1:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
       <c r="E3" s="62"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
-      <c r="H3" s="91">
+      <c r="H3" s="85">
         <v>41076</v>
       </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="89"/>
-      <c r="T3" s="89"/>
-      <c r="U3" s="89"/>
-      <c r="V3" s="89"/>
-      <c r="W3" s="89"/>
-      <c r="X3" s="89"/>
-      <c r="Y3" s="89"/>
-      <c r="Z3" s="89"/>
-      <c r="AA3" s="89"/>
-      <c r="AB3" s="89"/>
-      <c r="AC3" s="89"/>
-      <c r="AD3" s="89"/>
-      <c r="AE3" s="90"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="83"/>
+      <c r="S3" s="83"/>
+      <c r="T3" s="83"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="83"/>
+      <c r="AA3" s="83"/>
+      <c r="AB3" s="83"/>
+      <c r="AC3" s="83"/>
+      <c r="AD3" s="83"/>
+      <c r="AE3" s="84"/>
     </row>
     <row r="4" spans="1:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
       <c r="F4" s="61"/>
       <c r="G4" s="61"/>
-      <c r="H4" s="88" t="s">
+      <c r="H4" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="89"/>
-      <c r="W4" s="89"/>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="89"/>
-      <c r="AD4" s="89"/>
-      <c r="AE4" s="90"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="83"/>
+      <c r="U4" s="83"/>
+      <c r="V4" s="83"/>
+      <c r="W4" s="83"/>
+      <c r="X4" s="83"/>
+      <c r="Y4" s="83"/>
+      <c r="Z4" s="83"/>
+      <c r="AA4" s="83"/>
+      <c r="AB4" s="83"/>
+      <c r="AC4" s="83"/>
+      <c r="AD4" s="83"/>
+      <c r="AE4" s="84"/>
     </row>
     <row r="5" spans="1:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
+      <c r="A5" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
       <c r="F5" s="61"/>
       <c r="G5" s="61"/>
-      <c r="H5" s="88" t="s">
+      <c r="H5" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="89"/>
-      <c r="S5" s="89"/>
-      <c r="T5" s="89"/>
-      <c r="U5" s="89"/>
-      <c r="V5" s="89"/>
-      <c r="W5" s="89"/>
-      <c r="X5" s="89"/>
-      <c r="Y5" s="89"/>
-      <c r="Z5" s="89"/>
-      <c r="AA5" s="89"/>
-      <c r="AB5" s="89"/>
-      <c r="AC5" s="89"/>
-      <c r="AD5" s="89"/>
-      <c r="AE5" s="90"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="83"/>
+      <c r="Q5" s="83"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="83"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="83"/>
+      <c r="AA5" s="83"/>
+      <c r="AB5" s="83"/>
+      <c r="AC5" s="83"/>
+      <c r="AD5" s="83"/>
+      <c r="AE5" s="84"/>
     </row>
     <row r="6" spans="1:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="78" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="78"/>
-      <c r="R6" s="78"/>
-      <c r="S6" s="78"/>
-      <c r="T6" s="78"/>
-      <c r="U6" s="78"/>
-      <c r="V6" s="78"/>
-      <c r="W6" s="78"/>
-      <c r="X6" s="78"/>
-      <c r="Y6" s="78"/>
-      <c r="Z6" s="78"/>
-      <c r="AA6" s="78"/>
-      <c r="AB6" s="78"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="79"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="X6" s="79"/>
+      <c r="Y6" s="79"/>
+      <c r="Z6" s="79"/>
+      <c r="AA6" s="79"/>
+      <c r="AB6" s="79"/>
     </row>
     <row r="7" spans="1:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="87" t="s">
         <v>627</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="80"/>
-      <c r="P7" s="80"/>
-      <c r="Q7" s="80"/>
-      <c r="R7" s="80"/>
-      <c r="S7" s="80"/>
-      <c r="T7" s="80"/>
-      <c r="U7" s="80"/>
-      <c r="V7" s="80"/>
-      <c r="W7" s="80"/>
-      <c r="X7" s="80"/>
-      <c r="Y7" s="80"/>
-      <c r="Z7" s="80"/>
-      <c r="AA7" s="80"/>
-      <c r="AB7" s="80"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="88"/>
+      <c r="L7" s="88"/>
+      <c r="M7" s="88"/>
+      <c r="N7" s="88"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="88"/>
+      <c r="R7" s="88"/>
+      <c r="S7" s="88"/>
+      <c r="T7" s="88"/>
+      <c r="U7" s="88"/>
+      <c r="V7" s="88"/>
+      <c r="W7" s="88"/>
+      <c r="X7" s="88"/>
+      <c r="Y7" s="88"/>
+      <c r="Z7" s="88"/>
+      <c r="AA7" s="88"/>
+      <c r="AB7" s="88"/>
     </row>
     <row r="8" spans="1:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="78"/>
-      <c r="S8" s="78"/>
-      <c r="T8" s="78"/>
-      <c r="U8" s="78"/>
-      <c r="V8" s="78"/>
-      <c r="W8" s="78"/>
-      <c r="X8" s="78"/>
-      <c r="Y8" s="78"/>
-      <c r="Z8" s="78"/>
-      <c r="AA8" s="78"/>
-      <c r="AB8" s="78"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="79"/>
+      <c r="N8" s="79"/>
+      <c r="O8" s="79"/>
+      <c r="P8" s="79"/>
+      <c r="Q8" s="79"/>
+      <c r="R8" s="79"/>
+      <c r="S8" s="79"/>
+      <c r="T8" s="79"/>
+      <c r="U8" s="79"/>
+      <c r="V8" s="79"/>
+      <c r="W8" s="79"/>
+      <c r="X8" s="79"/>
+      <c r="Y8" s="79"/>
+      <c r="Z8" s="79"/>
+      <c r="AA8" s="79"/>
+      <c r="AB8" s="79"/>
     </row>
     <row r="9" spans="1:31" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="76"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="76"/>
-      <c r="S9" s="76"/>
-      <c r="T9" s="76"/>
-      <c r="U9" s="76"/>
-      <c r="V9" s="76"/>
-      <c r="W9" s="76"/>
-      <c r="X9" s="76"/>
-      <c r="Y9" s="76"/>
-      <c r="Z9" s="76"/>
-      <c r="AA9" s="76"/>
-      <c r="AB9" s="76"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="86"/>
+      <c r="R9" s="86"/>
+      <c r="S9" s="86"/>
+      <c r="T9" s="86"/>
+      <c r="U9" s="86"/>
+      <c r="V9" s="86"/>
+      <c r="W9" s="86"/>
+      <c r="X9" s="86"/>
+      <c r="Y9" s="86"/>
+      <c r="Z9" s="86"/>
+      <c r="AA9" s="86"/>
+      <c r="AB9" s="86"/>
     </row>
     <row r="10" spans="1:31" s="68" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="63" t="s">
@@ -14533,41 +14564,41 @@
     </row>
     <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A75" s="46"/>
-      <c r="B75" s="83" t="s">
+      <c r="B75" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="C75" s="84"/>
-      <c r="D75" s="84"/>
-      <c r="E75" s="84" t="s">
+      <c r="C75" s="90"/>
+      <c r="D75" s="90"/>
+      <c r="E75" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="F75" s="84"/>
-      <c r="G75" s="84"/>
-      <c r="H75" s="84"/>
-      <c r="I75" s="84" t="s">
+      <c r="F75" s="90"/>
+      <c r="G75" s="90"/>
+      <c r="H75" s="90"/>
+      <c r="I75" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="J75" s="84"/>
-      <c r="K75" s="84"/>
-      <c r="L75" s="84"/>
-      <c r="M75" s="84"/>
-      <c r="N75" s="84"/>
-      <c r="O75" s="84"/>
-      <c r="P75" s="84"/>
-      <c r="Q75" s="84"/>
-      <c r="R75" s="84"/>
-      <c r="S75" s="84" t="s">
+      <c r="J75" s="90"/>
+      <c r="K75" s="90"/>
+      <c r="L75" s="90"/>
+      <c r="M75" s="90"/>
+      <c r="N75" s="90"/>
+      <c r="O75" s="90"/>
+      <c r="P75" s="90"/>
+      <c r="Q75" s="90"/>
+      <c r="R75" s="90"/>
+      <c r="S75" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="T75" s="84"/>
-      <c r="U75" s="84"/>
-      <c r="V75" s="84"/>
-      <c r="W75" s="84"/>
-      <c r="X75" s="84"/>
-      <c r="Y75" s="84"/>
-      <c r="Z75" s="84"/>
-      <c r="AA75" s="84"/>
-      <c r="AB75" s="85"/>
+      <c r="T75" s="90"/>
+      <c r="U75" s="90"/>
+      <c r="V75" s="90"/>
+      <c r="W75" s="90"/>
+      <c r="X75" s="90"/>
+      <c r="Y75" s="90"/>
+      <c r="Z75" s="90"/>
+      <c r="AA75" s="90"/>
+      <c r="AB75" s="91"/>
       <c r="AC75" s="48"/>
       <c r="AD75" s="72"/>
     </row>
@@ -20549,6 +20580,15 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="E75:H75"/>
+    <mergeCell ref="I75:R75"/>
+    <mergeCell ref="S75:AB75"/>
+    <mergeCell ref="A9:AB9"/>
+    <mergeCell ref="A6:AB6"/>
+    <mergeCell ref="A7:AB7"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
     <mergeCell ref="A1:AB1"/>
     <mergeCell ref="A8:AB8"/>
     <mergeCell ref="A2:E2"/>
@@ -20557,15 +20597,6 @@
     <mergeCell ref="H3:AE3"/>
     <mergeCell ref="H4:AE4"/>
     <mergeCell ref="H5:AE5"/>
-    <mergeCell ref="A9:AB9"/>
-    <mergeCell ref="A6:AB6"/>
-    <mergeCell ref="A7:AB7"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="E75:H75"/>
-    <mergeCell ref="I75:R75"/>
-    <mergeCell ref="S75:AB75"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20574,15 +20605,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ144"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F92" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="Y22" sqref="Y22"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -20597,329 +20628,329 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
-      <c r="AD1" s="87"/>
-      <c r="AE1" s="97"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="93"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="88" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
-      <c r="V2" s="89"/>
-      <c r="W2" s="89"/>
-      <c r="X2" s="89"/>
-      <c r="Y2" s="89"/>
-      <c r="Z2" s="89"/>
-      <c r="AA2" s="89"/>
-      <c r="AB2" s="89"/>
-      <c r="AC2" s="89"/>
-      <c r="AD2" s="89"/>
-      <c r="AE2" s="90"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="83"/>
+      <c r="W2" s="83"/>
+      <c r="X2" s="83"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="83"/>
+      <c r="AA2" s="83"/>
+      <c r="AB2" s="83"/>
+      <c r="AC2" s="83"/>
+      <c r="AD2" s="83"/>
+      <c r="AE2" s="84"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="91">
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="85">
         <v>41086</v>
       </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="89"/>
-      <c r="T3" s="89"/>
-      <c r="U3" s="89"/>
-      <c r="V3" s="89"/>
-      <c r="W3" s="89"/>
-      <c r="X3" s="89"/>
-      <c r="Y3" s="89"/>
-      <c r="Z3" s="89"/>
-      <c r="AA3" s="89"/>
-      <c r="AB3" s="89"/>
-      <c r="AC3" s="89"/>
-      <c r="AD3" s="89"/>
-      <c r="AE3" s="90"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="83"/>
+      <c r="S3" s="83"/>
+      <c r="T3" s="83"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="83"/>
+      <c r="AA3" s="83"/>
+      <c r="AB3" s="83"/>
+      <c r="AC3" s="83"/>
+      <c r="AD3" s="83"/>
+      <c r="AE3" s="84"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="88" t="s">
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="89"/>
-      <c r="W4" s="89"/>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="89"/>
-      <c r="AD4" s="89"/>
-      <c r="AE4" s="90"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="83"/>
+      <c r="U4" s="83"/>
+      <c r="V4" s="83"/>
+      <c r="W4" s="83"/>
+      <c r="X4" s="83"/>
+      <c r="Y4" s="83"/>
+      <c r="Z4" s="83"/>
+      <c r="AA4" s="83"/>
+      <c r="AB4" s="83"/>
+      <c r="AC4" s="83"/>
+      <c r="AD4" s="83"/>
+      <c r="AE4" s="84"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="93" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="88" t="s">
+      <c r="A5" s="94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="89"/>
-      <c r="S5" s="89"/>
-      <c r="T5" s="89"/>
-      <c r="U5" s="89"/>
-      <c r="V5" s="89"/>
-      <c r="W5" s="89"/>
-      <c r="X5" s="89"/>
-      <c r="Y5" s="89"/>
-      <c r="Z5" s="89"/>
-      <c r="AA5" s="89"/>
-      <c r="AB5" s="89"/>
-      <c r="AC5" s="89"/>
-      <c r="AD5" s="89"/>
-      <c r="AE5" s="90"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="83"/>
+      <c r="Q5" s="83"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="83"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="83"/>
+      <c r="AA5" s="83"/>
+      <c r="AB5" s="83"/>
+      <c r="AC5" s="83"/>
+      <c r="AD5" s="83"/>
+      <c r="AE5" s="84"/>
     </row>
     <row r="6" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="78"/>
-      <c r="R6" s="78"/>
-      <c r="S6" s="78"/>
-      <c r="T6" s="78"/>
-      <c r="U6" s="78"/>
-      <c r="V6" s="78"/>
-      <c r="W6" s="78"/>
-      <c r="X6" s="78"/>
-      <c r="Y6" s="78"/>
-      <c r="Z6" s="78"/>
-      <c r="AA6" s="78"/>
-      <c r="AB6" s="78"/>
-      <c r="AC6" s="78"/>
-      <c r="AD6" s="78"/>
-      <c r="AE6" s="95"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="79"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="X6" s="79"/>
+      <c r="Y6" s="79"/>
+      <c r="Z6" s="79"/>
+      <c r="AA6" s="79"/>
+      <c r="AB6" s="79"/>
+      <c r="AC6" s="79"/>
+      <c r="AD6" s="79"/>
+      <c r="AE6" s="92"/>
     </row>
     <row r="7" spans="1:35" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="87" t="s">
         <v>215</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="80"/>
-      <c r="P7" s="80"/>
-      <c r="Q7" s="80"/>
-      <c r="R7" s="80"/>
-      <c r="S7" s="80"/>
-      <c r="T7" s="80"/>
-      <c r="U7" s="80"/>
-      <c r="V7" s="80"/>
-      <c r="W7" s="80"/>
-      <c r="X7" s="80"/>
-      <c r="Y7" s="80"/>
-      <c r="Z7" s="80"/>
-      <c r="AA7" s="80"/>
-      <c r="AB7" s="80"/>
-      <c r="AC7" s="80"/>
-      <c r="AD7" s="80"/>
-      <c r="AE7" s="96"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="88"/>
+      <c r="L7" s="88"/>
+      <c r="M7" s="88"/>
+      <c r="N7" s="88"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="88"/>
+      <c r="R7" s="88"/>
+      <c r="S7" s="88"/>
+      <c r="T7" s="88"/>
+      <c r="U7" s="88"/>
+      <c r="V7" s="88"/>
+      <c r="W7" s="88"/>
+      <c r="X7" s="88"/>
+      <c r="Y7" s="88"/>
+      <c r="Z7" s="88"/>
+      <c r="AA7" s="88"/>
+      <c r="AB7" s="88"/>
+      <c r="AC7" s="88"/>
+      <c r="AD7" s="88"/>
+      <c r="AE7" s="97"/>
     </row>
     <row r="8" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="78"/>
-      <c r="S8" s="78"/>
-      <c r="T8" s="78"/>
-      <c r="U8" s="78"/>
-      <c r="V8" s="78"/>
-      <c r="W8" s="78"/>
-      <c r="X8" s="78"/>
-      <c r="Y8" s="78"/>
-      <c r="Z8" s="78"/>
-      <c r="AA8" s="78"/>
-      <c r="AB8" s="78"/>
-      <c r="AC8" s="78"/>
-      <c r="AD8" s="78"/>
-      <c r="AE8" s="95"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="79"/>
+      <c r="N8" s="79"/>
+      <c r="O8" s="79"/>
+      <c r="P8" s="79"/>
+      <c r="Q8" s="79"/>
+      <c r="R8" s="79"/>
+      <c r="S8" s="79"/>
+      <c r="T8" s="79"/>
+      <c r="U8" s="79"/>
+      <c r="V8" s="79"/>
+      <c r="W8" s="79"/>
+      <c r="X8" s="79"/>
+      <c r="Y8" s="79"/>
+      <c r="Z8" s="79"/>
+      <c r="AA8" s="79"/>
+      <c r="AB8" s="79"/>
+      <c r="AC8" s="79"/>
+      <c r="AD8" s="79"/>
+      <c r="AE8" s="92"/>
     </row>
     <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="76"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="76"/>
-      <c r="S9" s="76"/>
-      <c r="T9" s="76"/>
-      <c r="U9" s="76"/>
-      <c r="V9" s="76"/>
-      <c r="W9" s="76"/>
-      <c r="X9" s="76"/>
-      <c r="Y9" s="76"/>
-      <c r="Z9" s="76"/>
-      <c r="AA9" s="76"/>
-      <c r="AB9" s="76"/>
-      <c r="AC9" s="76"/>
-      <c r="AD9" s="76"/>
-      <c r="AE9" s="76"/>
-    </row>
-    <row r="10" spans="1:35" s="42" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="86"/>
+      <c r="R9" s="86"/>
+      <c r="S9" s="86"/>
+      <c r="T9" s="86"/>
+      <c r="U9" s="86"/>
+      <c r="V9" s="86"/>
+      <c r="W9" s="86"/>
+      <c r="X9" s="86"/>
+      <c r="Y9" s="86"/>
+      <c r="Z9" s="86"/>
+      <c r="AA9" s="86"/>
+      <c r="AB9" s="86"/>
+      <c r="AC9" s="86"/>
+      <c r="AD9" s="86"/>
+      <c r="AE9" s="86"/>
+    </row>
+    <row r="10" spans="1:35" s="42" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="39" t="s">
         <v>72</v>
       </c>
@@ -20950,8 +20981,8 @@
       <c r="J10" s="40" t="s">
         <v>604</v>
       </c>
-      <c r="K10" s="39">
-        <v>1</v>
+      <c r="K10" s="117" t="s">
+        <v>645</v>
       </c>
       <c r="L10" s="39" t="s">
         <v>605</v>
@@ -27748,45 +27779,45 @@
     </row>
     <row r="75" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="46"/>
-      <c r="B75" s="83" t="s">
+      <c r="B75" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="C75" s="84"/>
-      <c r="D75" s="84" t="s">
+      <c r="C75" s="90"/>
+      <c r="D75" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="E75" s="84"/>
-      <c r="F75" s="84"/>
-      <c r="G75" s="84"/>
-      <c r="H75" s="84"/>
-      <c r="I75" s="84" t="s">
+      <c r="E75" s="90"/>
+      <c r="F75" s="90"/>
+      <c r="G75" s="90"/>
+      <c r="H75" s="90"/>
+      <c r="I75" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="J75" s="84"/>
-      <c r="K75" s="84"/>
-      <c r="L75" s="84"/>
-      <c r="M75" s="84"/>
-      <c r="N75" s="84"/>
-      <c r="O75" s="94"/>
-      <c r="P75" s="84"/>
-      <c r="Q75" s="84"/>
-      <c r="R75" s="84" t="s">
+      <c r="J75" s="90"/>
+      <c r="K75" s="90"/>
+      <c r="L75" s="90"/>
+      <c r="M75" s="90"/>
+      <c r="N75" s="90"/>
+      <c r="O75" s="96"/>
+      <c r="P75" s="90"/>
+      <c r="Q75" s="90"/>
+      <c r="R75" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="S75" s="84"/>
-      <c r="T75" s="84"/>
-      <c r="U75" s="84"/>
-      <c r="V75" s="84"/>
-      <c r="W75" s="84"/>
-      <c r="X75" s="84"/>
-      <c r="Y75" s="84"/>
-      <c r="Z75" s="84"/>
-      <c r="AA75" s="84"/>
-      <c r="AB75" s="84"/>
-      <c r="AC75" s="84"/>
-      <c r="AD75" s="84"/>
-      <c r="AE75" s="84"/>
-      <c r="AF75" s="84"/>
+      <c r="S75" s="90"/>
+      <c r="T75" s="90"/>
+      <c r="U75" s="90"/>
+      <c r="V75" s="90"/>
+      <c r="W75" s="90"/>
+      <c r="X75" s="90"/>
+      <c r="Y75" s="90"/>
+      <c r="Z75" s="90"/>
+      <c r="AA75" s="90"/>
+      <c r="AB75" s="90"/>
+      <c r="AC75" s="90"/>
+      <c r="AD75" s="90"/>
+      <c r="AE75" s="90"/>
+      <c r="AF75" s="90"/>
       <c r="AG75" s="47" t="s">
         <v>85</v>
       </c>
@@ -28002,40 +28033,40 @@
       </c>
     </row>
     <row r="78" spans="1:36" s="51" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="92" t="s">
+      <c r="B78" s="95" t="s">
         <v>87</v>
       </c>
-      <c r="C78" s="92"/>
-      <c r="D78" s="92"/>
-      <c r="E78" s="92"/>
-      <c r="F78" s="92"/>
-      <c r="G78" s="92"/>
-      <c r="H78" s="92"/>
-      <c r="I78" s="92"/>
-      <c r="J78" s="92"/>
-      <c r="K78" s="92"/>
-      <c r="L78" s="92"/>
-      <c r="M78" s="92"/>
-      <c r="N78" s="92"/>
-      <c r="O78" s="92"/>
-      <c r="P78" s="92"/>
-      <c r="Q78" s="92"/>
-      <c r="R78" s="92"/>
-      <c r="S78" s="92"/>
-      <c r="T78" s="92"/>
-      <c r="U78" s="92"/>
-      <c r="V78" s="92"/>
-      <c r="W78" s="92"/>
-      <c r="X78" s="92"/>
-      <c r="Y78" s="92"/>
-      <c r="Z78" s="92"/>
-      <c r="AA78" s="92"/>
-      <c r="AB78" s="92"/>
-      <c r="AC78" s="92"/>
-      <c r="AD78" s="92"/>
-      <c r="AE78" s="92"/>
-      <c r="AF78" s="92"/>
-      <c r="AG78" s="92"/>
+      <c r="C78" s="95"/>
+      <c r="D78" s="95"/>
+      <c r="E78" s="95"/>
+      <c r="F78" s="95"/>
+      <c r="G78" s="95"/>
+      <c r="H78" s="95"/>
+      <c r="I78" s="95"/>
+      <c r="J78" s="95"/>
+      <c r="K78" s="95"/>
+      <c r="L78" s="95"/>
+      <c r="M78" s="95"/>
+      <c r="N78" s="95"/>
+      <c r="O78" s="95"/>
+      <c r="P78" s="95"/>
+      <c r="Q78" s="95"/>
+      <c r="R78" s="95"/>
+      <c r="S78" s="95"/>
+      <c r="T78" s="95"/>
+      <c r="U78" s="95"/>
+      <c r="V78" s="95"/>
+      <c r="W78" s="95"/>
+      <c r="X78" s="95"/>
+      <c r="Y78" s="95"/>
+      <c r="Z78" s="95"/>
+      <c r="AA78" s="95"/>
+      <c r="AB78" s="95"/>
+      <c r="AC78" s="95"/>
+      <c r="AD78" s="95"/>
+      <c r="AE78" s="95"/>
+      <c r="AF78" s="95"/>
+      <c r="AG78" s="95"/>
     </row>
     <row r="79" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K79" s="38" t="s">
@@ -34792,14 +34823,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A8:AE8"/>
-    <mergeCell ref="A9:AE9"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="H2:AE2"/>
-    <mergeCell ref="H3:AE3"/>
-    <mergeCell ref="H4:AE4"/>
-    <mergeCell ref="H5:AE5"/>
-    <mergeCell ref="A2:G2"/>
     <mergeCell ref="R75:AF75"/>
     <mergeCell ref="B78:AG78"/>
     <mergeCell ref="A3:G3"/>
@@ -34810,6 +34833,14 @@
     <mergeCell ref="I75:Q75"/>
     <mergeCell ref="A6:AE6"/>
     <mergeCell ref="A7:AE7"/>
+    <mergeCell ref="A8:AE8"/>
+    <mergeCell ref="A9:AE9"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="H2:AE2"/>
+    <mergeCell ref="H3:AE3"/>
+    <mergeCell ref="H4:AE4"/>
+    <mergeCell ref="H5:AE5"/>
+    <mergeCell ref="A2:G2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34818,7 +34849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AK143"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
@@ -34842,39 +34873,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="11.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="114"/>
-      <c r="R1" s="114"/>
-      <c r="S1" s="114"/>
-      <c r="T1" s="114"/>
-      <c r="U1" s="114"/>
-      <c r="V1" s="114"/>
-      <c r="W1" s="114"/>
-      <c r="X1" s="114"/>
-      <c r="Y1" s="114"/>
-      <c r="Z1" s="114"/>
-      <c r="AA1" s="114"/>
-      <c r="AB1" s="114"/>
-      <c r="AC1" s="114"/>
-      <c r="AD1" s="114"/>
-      <c r="AE1" s="115"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="103"/>
+      <c r="W1" s="103"/>
+      <c r="X1" s="103"/>
+      <c r="Y1" s="103"/>
+      <c r="Z1" s="103"/>
+      <c r="AA1" s="103"/>
+      <c r="AB1" s="103"/>
+      <c r="AC1" s="103"/>
+      <c r="AD1" s="103"/>
+      <c r="AE1" s="104"/>
     </row>
     <row r="2" spans="1:36" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A2" s="98" t="s">
@@ -34923,7 +34954,7 @@
       <c r="E3" s="98"/>
       <c r="F3" s="98"/>
       <c r="G3" s="98"/>
-      <c r="H3" s="116">
+      <c r="H3" s="105">
         <v>41088</v>
       </c>
       <c r="I3" s="100"/>
@@ -35025,144 +35056,144 @@
       <c r="AE5" s="101"/>
     </row>
     <row r="6" spans="1:36" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="106" t="s">
         <v>569</v>
       </c>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103"/>
-      <c r="N6" s="103"/>
-      <c r="O6" s="103"/>
-      <c r="P6" s="103"/>
-      <c r="Q6" s="103"/>
-      <c r="R6" s="103"/>
-      <c r="S6" s="103"/>
-      <c r="T6" s="103"/>
-      <c r="U6" s="103"/>
-      <c r="V6" s="103"/>
-      <c r="W6" s="103"/>
-      <c r="X6" s="103"/>
-      <c r="Y6" s="103"/>
-      <c r="Z6" s="103"/>
-      <c r="AA6" s="103"/>
-      <c r="AB6" s="103"/>
-      <c r="AC6" s="103"/>
-      <c r="AD6" s="103"/>
-      <c r="AE6" s="104"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="107"/>
+      <c r="M6" s="107"/>
+      <c r="N6" s="107"/>
+      <c r="O6" s="107"/>
+      <c r="P6" s="107"/>
+      <c r="Q6" s="107"/>
+      <c r="R6" s="107"/>
+      <c r="S6" s="107"/>
+      <c r="T6" s="107"/>
+      <c r="U6" s="107"/>
+      <c r="V6" s="107"/>
+      <c r="W6" s="107"/>
+      <c r="X6" s="107"/>
+      <c r="Y6" s="107"/>
+      <c r="Z6" s="107"/>
+      <c r="AA6" s="107"/>
+      <c r="AB6" s="107"/>
+      <c r="AC6" s="107"/>
+      <c r="AD6" s="107"/>
+      <c r="AE6" s="108"/>
     </row>
     <row r="7" spans="1:36" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="109" t="s">
+      <c r="A7" s="113" t="s">
         <v>570</v>
       </c>
-      <c r="B7" s="110"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
-      <c r="L7" s="110"/>
-      <c r="M7" s="110"/>
-      <c r="N7" s="110"/>
-      <c r="O7" s="110"/>
-      <c r="P7" s="110"/>
-      <c r="Q7" s="110"/>
-      <c r="R7" s="110"/>
-      <c r="S7" s="110"/>
-      <c r="T7" s="110"/>
-      <c r="U7" s="110"/>
-      <c r="V7" s="110"/>
-      <c r="W7" s="110"/>
-      <c r="X7" s="110"/>
-      <c r="Y7" s="110"/>
-      <c r="Z7" s="110"/>
-      <c r="AA7" s="110"/>
-      <c r="AB7" s="110"/>
-      <c r="AC7" s="110"/>
-      <c r="AD7" s="110"/>
-      <c r="AE7" s="111"/>
+      <c r="B7" s="114"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114"/>
+      <c r="K7" s="114"/>
+      <c r="L7" s="114"/>
+      <c r="M7" s="114"/>
+      <c r="N7" s="114"/>
+      <c r="O7" s="114"/>
+      <c r="P7" s="114"/>
+      <c r="Q7" s="114"/>
+      <c r="R7" s="114"/>
+      <c r="S7" s="114"/>
+      <c r="T7" s="114"/>
+      <c r="U7" s="114"/>
+      <c r="V7" s="114"/>
+      <c r="W7" s="114"/>
+      <c r="X7" s="114"/>
+      <c r="Y7" s="114"/>
+      <c r="Z7" s="114"/>
+      <c r="AA7" s="114"/>
+      <c r="AB7" s="114"/>
+      <c r="AC7" s="114"/>
+      <c r="AD7" s="114"/>
+      <c r="AE7" s="115"/>
     </row>
     <row r="8" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="102" t="s">
+      <c r="A8" s="106" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="103"/>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="103"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103"/>
-      <c r="N8" s="103"/>
-      <c r="O8" s="103"/>
-      <c r="P8" s="103"/>
-      <c r="Q8" s="103"/>
-      <c r="R8" s="103"/>
-      <c r="S8" s="103"/>
-      <c r="T8" s="103"/>
-      <c r="U8" s="103"/>
-      <c r="V8" s="103"/>
-      <c r="W8" s="103"/>
-      <c r="X8" s="103"/>
-      <c r="Y8" s="103"/>
-      <c r="Z8" s="103"/>
-      <c r="AA8" s="103"/>
-      <c r="AB8" s="103"/>
-      <c r="AC8" s="103"/>
-      <c r="AD8" s="103"/>
-      <c r="AE8" s="104"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="107"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
+      <c r="K8" s="107"/>
+      <c r="L8" s="107"/>
+      <c r="M8" s="107"/>
+      <c r="N8" s="107"/>
+      <c r="O8" s="107"/>
+      <c r="P8" s="107"/>
+      <c r="Q8" s="107"/>
+      <c r="R8" s="107"/>
+      <c r="S8" s="107"/>
+      <c r="T8" s="107"/>
+      <c r="U8" s="107"/>
+      <c r="V8" s="107"/>
+      <c r="W8" s="107"/>
+      <c r="X8" s="107"/>
+      <c r="Y8" s="107"/>
+      <c r="Z8" s="107"/>
+      <c r="AA8" s="107"/>
+      <c r="AB8" s="107"/>
+      <c r="AC8" s="107"/>
+      <c r="AD8" s="107"/>
+      <c r="AE8" s="108"/>
     </row>
     <row r="9" spans="1:36" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="112"/>
-      <c r="C9" s="112"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="112"/>
-      <c r="H9" s="112"/>
-      <c r="I9" s="112"/>
-      <c r="J9" s="112"/>
-      <c r="K9" s="112"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="112"/>
-      <c r="N9" s="112"/>
-      <c r="O9" s="112"/>
-      <c r="P9" s="112"/>
-      <c r="Q9" s="112"/>
-      <c r="R9" s="112"/>
-      <c r="S9" s="112"/>
-      <c r="T9" s="112"/>
-      <c r="U9" s="112"/>
-      <c r="V9" s="112"/>
-      <c r="W9" s="112"/>
-      <c r="X9" s="112"/>
-      <c r="Y9" s="112"/>
-      <c r="Z9" s="112"/>
-      <c r="AA9" s="112"/>
-      <c r="AB9" s="112"/>
-      <c r="AC9" s="112"/>
-      <c r="AD9" s="112"/>
-      <c r="AE9" s="112"/>
+      <c r="B9" s="116"/>
+      <c r="C9" s="116"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="116"/>
+      <c r="H9" s="116"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="116"/>
+      <c r="M9" s="116"/>
+      <c r="N9" s="116"/>
+      <c r="O9" s="116"/>
+      <c r="P9" s="116"/>
+      <c r="Q9" s="116"/>
+      <c r="R9" s="116"/>
+      <c r="S9" s="116"/>
+      <c r="T9" s="116"/>
+      <c r="U9" s="116"/>
+      <c r="V9" s="116"/>
+      <c r="W9" s="116"/>
+      <c r="X9" s="116"/>
+      <c r="Y9" s="116"/>
+      <c r="Z9" s="116"/>
+      <c r="AA9" s="116"/>
+      <c r="AB9" s="116"/>
+      <c r="AC9" s="116"/>
+      <c r="AD9" s="116"/>
+      <c r="AE9" s="116"/>
     </row>
     <row r="10" spans="1:36" s="22" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
@@ -42190,43 +42221,43 @@
       <c r="B75" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C75" s="105" t="s">
+      <c r="C75" s="109" t="s">
         <v>79</v>
       </c>
-      <c r="D75" s="105"/>
-      <c r="E75" s="105"/>
-      <c r="F75" s="105"/>
-      <c r="G75" s="105"/>
-      <c r="H75" s="105"/>
-      <c r="I75" s="105"/>
-      <c r="J75" s="106" t="s">
+      <c r="D75" s="109"/>
+      <c r="E75" s="109"/>
+      <c r="F75" s="109"/>
+      <c r="G75" s="109"/>
+      <c r="H75" s="109"/>
+      <c r="I75" s="109"/>
+      <c r="J75" s="110" t="s">
         <v>82</v>
       </c>
-      <c r="K75" s="107"/>
-      <c r="L75" s="107"/>
-      <c r="M75" s="107"/>
-      <c r="N75" s="107"/>
-      <c r="O75" s="107"/>
-      <c r="P75" s="108"/>
-      <c r="Q75" s="105" t="s">
+      <c r="K75" s="111"/>
+      <c r="L75" s="111"/>
+      <c r="M75" s="111"/>
+      <c r="N75" s="111"/>
+      <c r="O75" s="111"/>
+      <c r="P75" s="112"/>
+      <c r="Q75" s="109" t="s">
         <v>83</v>
       </c>
-      <c r="R75" s="105"/>
-      <c r="S75" s="105"/>
-      <c r="T75" s="105"/>
-      <c r="U75" s="105"/>
-      <c r="V75" s="105"/>
-      <c r="W75" s="105"/>
-      <c r="X75" s="105"/>
-      <c r="Y75" s="105"/>
-      <c r="Z75" s="105"/>
-      <c r="AA75" s="105"/>
-      <c r="AB75" s="105"/>
-      <c r="AC75" s="105"/>
-      <c r="AD75" s="105"/>
-      <c r="AE75" s="105"/>
-      <c r="AF75" s="105"/>
-      <c r="AG75" s="105"/>
+      <c r="R75" s="109"/>
+      <c r="S75" s="109"/>
+      <c r="T75" s="109"/>
+      <c r="U75" s="109"/>
+      <c r="V75" s="109"/>
+      <c r="W75" s="109"/>
+      <c r="X75" s="109"/>
+      <c r="Y75" s="109"/>
+      <c r="Z75" s="109"/>
+      <c r="AA75" s="109"/>
+      <c r="AB75" s="109"/>
+      <c r="AC75" s="109"/>
+      <c r="AD75" s="109"/>
+      <c r="AE75" s="109"/>
+      <c r="AF75" s="109"/>
+      <c r="AG75" s="109"/>
       <c r="AH75" s="28" t="s">
         <v>84</v>
       </c>
@@ -49407,13 +49438,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="H4:AE4"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H2:AE2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="H3:AE3"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="H5:AE5"/>
     <mergeCell ref="A6:AE6"/>
@@ -49423,6 +49447,13 @@
     <mergeCell ref="A7:AE7"/>
     <mergeCell ref="A8:AE8"/>
     <mergeCell ref="A9:AE9"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="H4:AE4"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="H2:AE2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="H3:AE3"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.19685039370078741" right="0" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
@@ -49431,7 +49462,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G372"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -56203,6 +56234,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E0C724CCBB7FB24794473D558C897B81" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="86d9b256e064198c05d6efa412f72bef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="14f82cd5-dea2-47e7-b602-401f39b9480a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9d018442e514e3a48a93ea56c159054e" ns2:_="">
     <xsd:import namespace="14f82cd5-dea2-47e7-b602-401f39b9480a"/>
@@ -56348,22 +56394,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{498E1E47-19AB-4689-AFBF-A9E7F3AC94EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58338D5B-5713-45A9-B1B3-B02B6F3E9B74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4BBC144-9A3F-4D7B-855B-83638B65E4AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -56379,21 +56427,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58338D5B-5713-45A9-B1B3-B02B6F3E9B74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{498E1E47-19AB-4689-AFBF-A9E7F3AC94EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>